<commit_message>
Added main files for major project parts.
</commit_message>
<xml_diff>
--- a/test_results/Subject_0.xlsx
+++ b/test_results/Subject_0.xlsx
@@ -14,165 +14,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="51">
   <si>
     <t>Complexity_3</t>
   </si>
   <si>
+    <t>LIVING_ROOM</t>
+  </si>
+  <si>
+    <t>HOA_Bin</t>
+  </si>
+  <si>
+    <t>same_room</t>
+  </si>
+  <si>
+    <t>SG4-SUSAN</t>
+  </si>
+  <si>
+    <t>STV-MARIA</t>
+  </si>
+  <si>
+    <t>S5-DAVID</t>
+  </si>
+  <si>
+    <t>Freeverb</t>
+  </si>
+  <si>
+    <t>SG4-DAVID</t>
+  </si>
+  <si>
+    <t>S5-SUSAN</t>
+  </si>
+  <si>
+    <t>METU</t>
+  </si>
+  <si>
+    <t>302-MARIA</t>
+  </si>
+  <si>
+    <t>032-SUSAN</t>
+  </si>
+  <si>
+    <t>152-DAVID</t>
+  </si>
+  <si>
+    <t>302-SUSAN</t>
+  </si>
+  <si>
+    <t>032-DAVID</t>
+  </si>
+  <si>
+    <t>152-MARIA</t>
+  </si>
+  <si>
+    <t>3D_MARCo</t>
+  </si>
+  <si>
+    <t>+30-DAVID</t>
+  </si>
+  <si>
+    <t>0-SUSAN</t>
+  </si>
+  <si>
+    <t>-90-MARIA</t>
+  </si>
+  <si>
+    <t>-90-ALEX</t>
+  </si>
+  <si>
     <t>AALBORG</t>
   </si>
   <si>
-    <t>HOA_Bin</t>
-  </si>
-  <si>
-    <t>same_room</t>
+    <t>-60-MARIA</t>
+  </si>
+  <si>
+    <t>+30-MARIA</t>
+  </si>
+  <si>
+    <t>0-DAVID</t>
+  </si>
+  <si>
+    <t>-60-SUSAN</t>
+  </si>
+  <si>
+    <t>Complexity_2</t>
+  </si>
+  <si>
+    <t>-90-SUSAN</t>
+  </si>
+  <si>
+    <t>+30-ALEX</t>
+  </si>
+  <si>
+    <t>S5-ALEX</t>
+  </si>
+  <si>
+    <t>302-DAVID</t>
+  </si>
+  <si>
+    <t>032-ALEX</t>
+  </si>
+  <si>
+    <t>032-MARIA</t>
+  </si>
+  <si>
+    <t>Complexity_4</t>
+  </si>
+  <si>
+    <t>-30-MARIA</t>
   </si>
   <si>
     <t>+30-SUSAN</t>
   </si>
   <si>
-    <t>0-DAVID</t>
-  </si>
-  <si>
-    <t>-60-MARIA</t>
-  </si>
-  <si>
-    <t>Freeverb</t>
-  </si>
-  <si>
-    <t>+30-RICHARD</t>
-  </si>
-  <si>
-    <t>0-MARIA</t>
-  </si>
-  <si>
-    <t>-60-DAVID</t>
-  </si>
-  <si>
-    <t>METU</t>
-  </si>
-  <si>
-    <t>302-DAVID</t>
-  </si>
-  <si>
-    <t>032-RICHARD</t>
-  </si>
-  <si>
-    <t>152-MARIA</t>
-  </si>
-  <si>
-    <t>302-MARIA</t>
-  </si>
-  <si>
-    <t>032-DAVID</t>
-  </si>
-  <si>
-    <t>152-RICHARD</t>
-  </si>
-  <si>
-    <t>3D_MARCo</t>
-  </si>
-  <si>
-    <t>0-RICHARD</t>
-  </si>
-  <si>
-    <t>-90-MARIA</t>
-  </si>
-  <si>
-    <t>-90-DAVID</t>
-  </si>
-  <si>
-    <t>LIVING_ROOM</t>
-  </si>
-  <si>
-    <t>SG4-SUSAN</t>
-  </si>
-  <si>
-    <t>STV-MARIA</t>
-  </si>
-  <si>
-    <t>S5-DAVID</t>
-  </si>
-  <si>
-    <t>SG4-RICHARD</t>
+    <t>0-ALEX</t>
+  </si>
+  <si>
+    <t>-30-DAVID</t>
+  </si>
+  <si>
+    <t>SG6-SUSAN</t>
+  </si>
+  <si>
+    <t>SG4-MARIA</t>
+  </si>
+  <si>
+    <t>STV-ALEX</t>
+  </si>
+  <si>
+    <t>SG6-MARIA</t>
+  </si>
+  <si>
+    <t>SG4-ALEX</t>
   </si>
   <si>
     <t>STV-SUSAN</t>
   </si>
   <si>
-    <t>S5-MARIA</t>
-  </si>
-  <si>
-    <t>Complexity_2</t>
-  </si>
-  <si>
-    <t>032-MARIA</t>
-  </si>
-  <si>
-    <t>-60-RICHARD</t>
-  </si>
-  <si>
-    <t>+30-MARIA</t>
-  </si>
-  <si>
-    <t>-90-RICHARD</t>
-  </si>
-  <si>
-    <t>SG4-DAVID</t>
-  </si>
-  <si>
-    <t>Complexity_4</t>
-  </si>
-  <si>
-    <t>+30-DAVID</t>
-  </si>
-  <si>
-    <t>-30-SUSAN</t>
-  </si>
-  <si>
-    <t>-90-SUSAN</t>
-  </si>
-  <si>
-    <t>-30-DAVID</t>
-  </si>
-  <si>
-    <t>302-SUSAN</t>
-  </si>
-  <si>
-    <t>112-MARIA</t>
+    <t>+120-SUSAN</t>
+  </si>
+  <si>
+    <t>-60-ALEX</t>
+  </si>
+  <si>
+    <t>+120-ALEX</t>
+  </si>
+  <si>
+    <t>302-ALEX</t>
   </si>
   <si>
     <t>112-SUSAN</t>
   </si>
   <si>
-    <t>152-DAVID</t>
-  </si>
-  <si>
-    <t>SG6-SUSAN</t>
-  </si>
-  <si>
-    <t>SG4-MARIA</t>
-  </si>
-  <si>
-    <t>STV-DAVID</t>
-  </si>
-  <si>
-    <t>S5-RICHARD</t>
-  </si>
-  <si>
-    <t>SG6-MARIA</t>
-  </si>
-  <si>
-    <t>S5-SUSAN</t>
-  </si>
-  <si>
-    <t>+120-RICHARD</t>
-  </si>
-  <si>
-    <t>0-SUSAN</t>
-  </si>
-  <si>
-    <t>+120-MARIA</t>
+    <t>152-ALEX</t>
   </si>
 </sst>
 </file>
@@ -211,7 +205,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF800080"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +217,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF800080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,11 +602,11 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -622,11 +616,11 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -636,11 +630,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -664,39 +658,39 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="4" t="s">
-        <v>36</v>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="6" t="s">
-        <v>9</v>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="5" t="s">
-        <v>33</v>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -709,8 +703,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
+      <c r="E8" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -719,22 +713,22 @@
         <v>3</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
@@ -743,58 +737,58 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
+      <c r="A11" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="5" t="s">
-        <v>8</v>
+      <c r="E11" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
+      <c r="A12" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="6" t="s">
-        <v>9</v>
+      <c r="E12" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="3" t="s">
-        <v>38</v>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="4" t="s">
-        <v>39</v>
+      <c r="E14" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -803,18 +797,18 @@
         <v>3</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
@@ -822,13 +816,13 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="5" t="s">
-        <v>13</v>
+      <c r="A17" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -842,29 +836,29 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
+      <c r="C18" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -874,31 +868,31 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="4" t="s">
-        <v>16</v>
+      <c r="E20" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="5" t="s">
-        <v>17</v>
+      <c r="E21" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
@@ -906,17 +900,17 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
@@ -926,15 +920,15 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="7" t="s">
-        <v>21</v>
+      <c r="C24" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="6" t="s">
-        <v>15</v>
+      <c r="E24" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -944,11 +938,11 @@
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="4" t="s">
-        <v>42</v>
+      <c r="E25" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -961,32 +955,32 @@
         <v>3</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="5" t="s">
-        <v>13</v>
+      <c r="E26" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="3" t="s">
-        <v>4</v>
+      <c r="A27" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="3" t="s">
-        <v>4</v>
+      <c r="C27" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="7" t="s">
-        <v>43</v>
+      <c r="E27" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
+      <c r="C28" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="1" t="s">
@@ -995,12 +989,12 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
@@ -1014,7 +1008,7 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
@@ -1032,49 +1026,49 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>4</v>
+      <c r="A32" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="4" t="s">
-        <v>23</v>
+      <c r="C32" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="6" t="s">
-        <v>45</v>
+      <c r="E32" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="7" t="s">
-        <v>46</v>
+      <c r="E33" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="4" t="s">
-        <v>47</v>
+      <c r="E34" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -1097,8 +1091,8 @@
         <v>2</v>
       </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="7" t="s">
-        <v>34</v>
+      <c r="C36" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
@@ -1112,41 +1106,41 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="6" t="s">
-        <v>48</v>
+      <c r="E37" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="3" t="s">
-        <v>23</v>
+      <c r="A38" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="E38" s="4" t="s">
-        <v>26</v>
+      <c r="E38" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="4" t="s">
-        <v>24</v>
+      <c r="A39" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B39" s="2"/>
       <c r="E39" s="7" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="7" t="s">
-        <v>25</v>
+      <c r="A40" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="E40" s="3" t="s">
-        <v>49</v>
+      <c r="E40" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -1156,7 +1150,7 @@
       </c>
       <c r="B41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -1171,8 +1165,8 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="4" t="s">
-        <v>26</v>
+      <c r="A43" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B43" s="2"/>
       <c r="E43" s="2" t="s">
@@ -1181,34 +1175,34 @@
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="3" t="s">
-        <v>27</v>
+      <c r="A44" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B44" s="2"/>
       <c r="E44" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="6" t="s">
-        <v>28</v>
+      <c r="A45" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="E45" s="6" t="s">
-        <v>32</v>
+      <c r="E45" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="E46" s="4" t="s">
-        <v>51</v>
+      <c r="E46" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6">
       <c r="E47" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -1225,26 +1219,26 @@
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="6" t="s">
-        <v>52</v>
+      <c r="E50" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="5:6">
-      <c r="E51" s="3" t="s">
-        <v>4</v>
+      <c r="E51" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="5:6">
-      <c r="E53" s="4" t="s">
-        <v>31</v>
+      <c r="E53" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="F53" s="2"/>
     </row>

</xml_diff>